<commit_message>
Remodelled after new Data prep  and new calc
</commit_message>
<xml_diff>
--- a/HR Analytics Case Study/calc.xlsx
+++ b/HR Analytics Case Study/calc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study Material\upgrad\logistic\PA-I_Case_Study_HR_Analytics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F351BD5-6070-48AE-A1A9-C5E2D0C6FAF0}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EED8F81F-93D8-4904-A1F2-F842EAAFCD34}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8664" xr2:uid="{CFB7CBD5-FE6F-4998-A73A-69D096A561DA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
   <si>
     <t>total</t>
   </si>
@@ -61,6 +61,12 @@
   </si>
   <si>
     <t>Cum Lift</t>
+  </si>
+  <si>
+    <t>OLD</t>
+  </si>
+  <si>
+    <t>NEW</t>
   </si>
 </sst>
 </file>
@@ -100,7 +106,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -243,11 +249,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -264,6 +288,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -578,10 +610,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1F7E994-205C-492C-839B-D0EC130FECB9}">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -591,471 +623,960 @@
     <col min="11" max="11" width="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:11" s="17" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K2" s="6" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="7">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>133</v>
-      </c>
-      <c r="C2" s="1">
-        <v>73</v>
-      </c>
-      <c r="D2" s="1">
-        <f>B2-C2</f>
-        <v>60</v>
-      </c>
-      <c r="E2" s="1">
-        <v>73</v>
-      </c>
-      <c r="F2" s="1">
-        <f>D2</f>
-        <v>60</v>
-      </c>
-      <c r="G2" s="1">
-        <v>34.700000000000003</v>
-      </c>
-      <c r="H2" s="1">
-        <v>3.43</v>
-      </c>
-      <c r="I2" s="2">
-        <f>E2/C$12</f>
-        <v>0.34272300469483569</v>
-      </c>
-      <c r="J2" s="2">
-        <f>F2/D$12</f>
-        <v>5.4054054054054057E-2</v>
-      </c>
-      <c r="K2" s="8">
-        <f>I2-J2</f>
-        <v>0.28866895064078163</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C3" s="1">
-        <v>41</v>
+        <v>73</v>
       </c>
       <c r="D3" s="1">
-        <f>B3-C3</f>
-        <v>91</v>
+        <f t="shared" ref="D3:D12" si="0">B3-C3</f>
+        <v>60</v>
       </c>
       <c r="E3" s="1">
-        <v>114</v>
+        <v>73</v>
       </c>
       <c r="F3" s="1">
-        <f>F2+D3</f>
-        <v>151</v>
+        <f>D3</f>
+        <v>60</v>
       </c>
       <c r="G3" s="1">
-        <v>53.5</v>
+        <v>34.700000000000003</v>
       </c>
       <c r="H3" s="1">
-        <v>2.68</v>
+        <v>3.43</v>
       </c>
       <c r="I3" s="2">
-        <f>E3/C$12</f>
-        <v>0.53521126760563376</v>
+        <f>E3/C$13</f>
+        <v>0.34272300469483569</v>
       </c>
       <c r="J3" s="2">
-        <f>F3/D$12</f>
-        <v>0.13603603603603603</v>
+        <f>F3/D$13</f>
+        <v>5.4054054054054057E-2</v>
       </c>
       <c r="K3" s="8">
-        <f>I3-J3</f>
-        <v>0.39917523156959772</v>
+        <f t="shared" ref="K3:K12" si="1">I3-J3</f>
+        <v>0.28866895064078163</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1">
         <v>132</v>
       </c>
       <c r="C4" s="1">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="D4" s="1">
-        <f>B4-C4</f>
-        <v>104</v>
+        <f t="shared" si="0"/>
+        <v>91</v>
       </c>
       <c r="E4" s="1">
-        <v>142</v>
+        <v>114</v>
       </c>
       <c r="F4" s="1">
-        <f>F3+D4</f>
-        <v>255</v>
-      </c>
-      <c r="G4" s="14">
-        <v>66.7</v>
-      </c>
-      <c r="H4" s="14">
-        <v>2.2200000000000002</v>
+        <f t="shared" ref="F4:F12" si="2">F3+D4</f>
+        <v>151</v>
+      </c>
+      <c r="G4" s="1">
+        <v>53.5</v>
+      </c>
+      <c r="H4" s="1">
+        <v>2.68</v>
       </c>
       <c r="I4" s="2">
-        <f>E4/C$12</f>
-        <v>0.66666666666666663</v>
+        <f>E4/C$13</f>
+        <v>0.53521126760563376</v>
       </c>
       <c r="J4" s="2">
-        <f>F4/D$12</f>
-        <v>0.22972972972972974</v>
-      </c>
-      <c r="K4" s="15">
-        <f>I4-J4</f>
-        <v>0.43693693693693691</v>
+        <f>F4/D$13</f>
+        <v>0.13603603603603603</v>
+      </c>
+      <c r="K4" s="8">
+        <f t="shared" si="1"/>
+        <v>0.39917523156959772</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C5" s="1">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="D5" s="1">
-        <f>B5-C5</f>
-        <v>116</v>
+        <f t="shared" si="0"/>
+        <v>104</v>
       </c>
       <c r="E5" s="1">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="F5" s="1">
-        <f>F4+D5</f>
-        <v>371</v>
-      </c>
-      <c r="G5" s="1">
-        <v>74.599999999999994</v>
-      </c>
-      <c r="H5" s="1">
-        <v>1.87</v>
+        <f t="shared" si="2"/>
+        <v>255</v>
+      </c>
+      <c r="G5" s="14">
+        <v>66.7</v>
+      </c>
+      <c r="H5" s="14">
+        <v>2.2200000000000002</v>
       </c>
       <c r="I5" s="2">
-        <f>E5/C$12</f>
-        <v>0.74647887323943662</v>
+        <f>E5/C$13</f>
+        <v>0.66666666666666663</v>
       </c>
       <c r="J5" s="2">
-        <f>F5/D$12</f>
-        <v>0.33423423423423421</v>
-      </c>
-      <c r="K5" s="8">
-        <f>I5-J5</f>
-        <v>0.41224463900520242</v>
+        <f>F5/D$13</f>
+        <v>0.22972972972972974</v>
+      </c>
+      <c r="K5" s="15">
+        <f t="shared" si="1"/>
+        <v>0.43693693693693691</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C6" s="1">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D6" s="1">
-        <f>B6-C6</f>
-        <v>109</v>
+        <f t="shared" si="0"/>
+        <v>116</v>
       </c>
       <c r="E6" s="1">
-        <v>182</v>
+        <v>159</v>
       </c>
       <c r="F6" s="1">
-        <f>F5+D6</f>
-        <v>480</v>
+        <f t="shared" si="2"/>
+        <v>371</v>
       </c>
       <c r="G6" s="1">
-        <v>85.4</v>
+        <v>74.599999999999994</v>
       </c>
       <c r="H6" s="1">
-        <v>1.71</v>
+        <v>1.87</v>
       </c>
       <c r="I6" s="2">
-        <f>E6/C$12</f>
-        <v>0.85446009389671362</v>
+        <f>E6/C$13</f>
+        <v>0.74647887323943662</v>
       </c>
       <c r="J6" s="2">
-        <f>F6/D$12</f>
-        <v>0.43243243243243246</v>
+        <f>F6/D$13</f>
+        <v>0.33423423423423421</v>
       </c>
       <c r="K6" s="8">
-        <f>I6-J6</f>
-        <v>0.42202766146428117</v>
+        <f t="shared" si="1"/>
+        <v>0.41224463900520242</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1">
         <v>132</v>
       </c>
       <c r="C7" s="1">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="D7" s="1">
-        <f>B7-C7</f>
-        <v>127</v>
+        <f t="shared" si="0"/>
+        <v>109</v>
       </c>
       <c r="E7" s="1">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="F7" s="1">
-        <f>F6+D7</f>
-        <v>607</v>
+        <f t="shared" si="2"/>
+        <v>480</v>
       </c>
       <c r="G7" s="1">
-        <v>87.8</v>
+        <v>85.4</v>
       </c>
       <c r="H7" s="1">
-        <v>1.46</v>
+        <v>1.71</v>
       </c>
       <c r="I7" s="2">
-        <f>E7/C$12</f>
-        <v>0.8779342723004695</v>
+        <f>E7/C$13</f>
+        <v>0.85446009389671362</v>
       </c>
       <c r="J7" s="2">
-        <f>F7/D$12</f>
-        <v>0.54684684684684681</v>
+        <f>F7/D$13</f>
+        <v>0.43243243243243246</v>
       </c>
       <c r="K7" s="8">
-        <f>I7-J7</f>
-        <v>0.33108742545362269</v>
+        <f t="shared" si="1"/>
+        <v>0.42202766146428117</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C8" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D8" s="1">
-        <f>B8-C8</f>
-        <v>125</v>
+        <f t="shared" si="0"/>
+        <v>127</v>
       </c>
       <c r="E8" s="1">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="F8" s="1">
-        <f>F7+D8</f>
-        <v>732</v>
+        <f t="shared" si="2"/>
+        <v>607</v>
       </c>
       <c r="G8" s="1">
-        <v>91.1</v>
+        <v>87.8</v>
       </c>
       <c r="H8" s="1">
-        <v>1.3</v>
+        <v>1.46</v>
       </c>
       <c r="I8" s="2">
-        <f>E8/C$12</f>
-        <v>0.91079812206572774</v>
+        <f>E8/C$13</f>
+        <v>0.8779342723004695</v>
       </c>
       <c r="J8" s="2">
-        <f>F8/D$12</f>
-        <v>0.6594594594594595</v>
+        <f>F8/D$13</f>
+        <v>0.54684684684684681</v>
       </c>
       <c r="K8" s="8">
-        <f>I8-J8</f>
-        <v>0.25133866260626825</v>
+        <f t="shared" si="1"/>
+        <v>0.33108742545362269</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="1">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C9" s="1">
         <v>8</v>
       </c>
       <c r="D9" s="1">
-        <f>B9-C9</f>
-        <v>124</v>
+        <f t="shared" si="0"/>
+        <v>125</v>
       </c>
       <c r="E9" s="1">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="F9" s="1">
-        <f>F8+D9</f>
-        <v>856</v>
+        <f t="shared" si="2"/>
+        <v>732</v>
       </c>
       <c r="G9" s="1">
-        <v>95.3</v>
+        <v>91.1</v>
       </c>
       <c r="H9" s="1">
-        <v>1.19</v>
+        <v>1.3</v>
       </c>
       <c r="I9" s="2">
-        <f>E9/C$12</f>
-        <v>0.95305164319248825</v>
+        <f>E9/C$13</f>
+        <v>0.91079812206572774</v>
       </c>
       <c r="J9" s="2">
-        <f>F9/D$12</f>
-        <v>0.77117117117117118</v>
+        <f>F9/D$13</f>
+        <v>0.6594594594594595</v>
       </c>
       <c r="K9" s="8">
-        <f>I9-J9</f>
-        <v>0.18188047202131707</v>
+        <f t="shared" si="1"/>
+        <v>0.25133866260626825</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="1">
         <v>132</v>
       </c>
       <c r="C10" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D10" s="1">
-        <f>B10-C10</f>
-        <v>125</v>
+        <f t="shared" si="0"/>
+        <v>124</v>
       </c>
       <c r="E10" s="1">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="F10" s="1">
-        <f>F9+D10</f>
-        <v>981</v>
+        <f t="shared" si="2"/>
+        <v>856</v>
       </c>
       <c r="G10" s="1">
-        <v>98.6</v>
+        <v>95.3</v>
       </c>
       <c r="H10" s="1">
-        <v>1.1000000000000001</v>
+        <v>1.19</v>
       </c>
       <c r="I10" s="2">
-        <f>E10/C$12</f>
-        <v>0.9859154929577465</v>
+        <f>E10/C$13</f>
+        <v>0.95305164319248825</v>
       </c>
       <c r="J10" s="2">
-        <f>F10/D$12</f>
-        <v>0.88378378378378375</v>
+        <f>F10/D$13</f>
+        <v>0.77117117117117118</v>
       </c>
       <c r="K10" s="8">
-        <f>I10-J10</f>
-        <v>0.10213170917396275</v>
+        <f t="shared" si="1"/>
+        <v>0.18188047202131707</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="7">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="1">
         <v>132</v>
       </c>
       <c r="C11" s="1">
+        <v>7</v>
+      </c>
+      <c r="D11" s="1">
+        <f t="shared" si="0"/>
+        <v>125</v>
+      </c>
+      <c r="E11" s="1">
+        <v>210</v>
+      </c>
+      <c r="F11" s="1">
+        <f t="shared" si="2"/>
+        <v>981</v>
+      </c>
+      <c r="G11" s="1">
+        <v>98.6</v>
+      </c>
+      <c r="H11" s="1">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="I11" s="2">
+        <f>E11/C$13</f>
+        <v>0.9859154929577465</v>
+      </c>
+      <c r="J11" s="2">
+        <f>F11/D$13</f>
+        <v>0.88378378378378375</v>
+      </c>
+      <c r="K11" s="8">
+        <f t="shared" si="1"/>
+        <v>0.10213170917396275</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="7">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1">
+        <v>132</v>
+      </c>
+      <c r="C12" s="1">
         <v>3</v>
       </c>
-      <c r="D11" s="1">
-        <f>B11-C11</f>
+      <c r="D12" s="1">
+        <f t="shared" si="0"/>
         <v>129</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E12" s="1">
         <v>213</v>
       </c>
-      <c r="F11" s="1">
-        <f>F10+D11</f>
+      <c r="F12" s="1">
+        <f t="shared" si="2"/>
         <v>1110</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G12" s="1">
         <v>100</v>
       </c>
-      <c r="H11" s="1">
+      <c r="H12" s="1">
         <v>1</v>
       </c>
-      <c r="I11" s="2">
-        <f>E11/C$12</f>
+      <c r="I12" s="2">
+        <f>E12/C$13</f>
         <v>1</v>
       </c>
-      <c r="J11" s="2">
-        <f>F11/D$12</f>
+      <c r="J12" s="2">
+        <f>F12/D$13</f>
         <v>1</v>
       </c>
-      <c r="K11" s="8">
-        <f>I11-J11</f>
+      <c r="K12" s="8">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="9" t="s">
+    <row r="13" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="10">
-        <f>SUM(B2:B11)</f>
+      <c r="B13" s="10">
+        <f>SUM(B3:B12)</f>
         <v>1323</v>
       </c>
-      <c r="C12" s="11">
-        <f>SUM(C2:C11)</f>
+      <c r="C13" s="11">
+        <f>SUM(C3:C12)</f>
         <v>213</v>
       </c>
-      <c r="D12" s="11">
-        <f>SUM(D2:D11)</f>
+      <c r="D13" s="11">
+        <f>SUM(D3:D12)</f>
         <v>1110</v>
       </c>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="13"/>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C19">
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="13"/>
+    </row>
+    <row r="17" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="18"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>1</v>
+      </c>
+      <c r="B19" s="1">
+        <v>133</v>
+      </c>
+      <c r="C19" s="1">
+        <v>77</v>
+      </c>
+      <c r="D19" s="1">
+        <f t="shared" ref="D19:D28" si="3">B19-C19</f>
+        <v>56</v>
+      </c>
+      <c r="E19" s="1">
+        <v>77</v>
+      </c>
+      <c r="F19" s="1">
+        <f>D19</f>
+        <v>56</v>
+      </c>
+      <c r="G19" s="1">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="H19" s="1">
+        <v>3.62</v>
+      </c>
+      <c r="I19" s="2">
+        <f>E19/C$13</f>
+        <v>0.36150234741784038</v>
+      </c>
+      <c r="J19" s="2">
+        <f>F19/D$13</f>
+        <v>5.0450450450450449E-2</v>
+      </c>
+      <c r="K19" s="2">
+        <f t="shared" ref="K19:K28" si="4">I19-J19</f>
+        <v>0.31105189696738994</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>2</v>
+      </c>
+      <c r="B20" s="1">
+        <v>132</v>
+      </c>
+      <c r="C20" s="1">
+        <v>39</v>
+      </c>
+      <c r="D20" s="1">
+        <f t="shared" si="3"/>
+        <v>93</v>
+      </c>
+      <c r="E20" s="1">
+        <v>116</v>
+      </c>
+      <c r="F20" s="1">
+        <f t="shared" ref="F20:F28" si="5">F19+D20</f>
+        <v>149</v>
+      </c>
+      <c r="G20" s="1">
+        <v>54.5</v>
+      </c>
+      <c r="H20" s="1">
+        <v>2.72</v>
+      </c>
+      <c r="I20" s="2">
+        <f>E20/C$13</f>
+        <v>0.54460093896713613</v>
+      </c>
+      <c r="J20" s="2">
+        <f>F20/D$13</f>
+        <v>0.13423423423423422</v>
+      </c>
+      <c r="K20" s="2">
+        <f t="shared" si="4"/>
+        <v>0.41036670473290193</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>3</v>
+      </c>
+      <c r="B21" s="1">
+        <v>132</v>
+      </c>
+      <c r="C21" s="1">
+        <v>26</v>
+      </c>
+      <c r="D21" s="1">
+        <f t="shared" si="3"/>
+        <v>106</v>
+      </c>
+      <c r="E21" s="1">
+        <v>142</v>
+      </c>
+      <c r="F21" s="1">
+        <f t="shared" si="5"/>
+        <v>255</v>
+      </c>
+      <c r="G21" s="14">
+        <v>66.7</v>
+      </c>
+      <c r="H21" s="14">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="I21" s="2">
+        <f>E21/C$13</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="J21" s="2">
+        <f>F21/D$13</f>
+        <v>0.22972972972972974</v>
+      </c>
+      <c r="K21" s="15">
+        <f t="shared" si="4"/>
+        <v>0.43693693693693691</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>4</v>
+      </c>
+      <c r="B22" s="1">
+        <v>133</v>
+      </c>
+      <c r="C22" s="1">
+        <v>19</v>
+      </c>
+      <c r="D22" s="1">
+        <f t="shared" si="3"/>
+        <v>114</v>
+      </c>
+      <c r="E22" s="1">
+        <v>161</v>
+      </c>
+      <c r="F22" s="1">
+        <f t="shared" si="5"/>
+        <v>369</v>
+      </c>
+      <c r="G22" s="1">
+        <v>75.599999999999994</v>
+      </c>
+      <c r="H22" s="1">
+        <v>1.89</v>
+      </c>
+      <c r="I22" s="2">
+        <f>E22/C$13</f>
+        <v>0.755868544600939</v>
+      </c>
+      <c r="J22" s="2">
+        <f>F22/D$13</f>
+        <v>0.33243243243243242</v>
+      </c>
+      <c r="K22" s="2">
+        <f t="shared" si="4"/>
+        <v>0.42343611216850657</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>5</v>
+      </c>
+      <c r="B23" s="1">
+        <v>132</v>
+      </c>
+      <c r="C23" s="1">
+        <v>16</v>
+      </c>
+      <c r="D23" s="1">
+        <f t="shared" si="3"/>
+        <v>116</v>
+      </c>
+      <c r="E23" s="1">
+        <v>177</v>
+      </c>
+      <c r="F23" s="1">
+        <f t="shared" si="5"/>
+        <v>485</v>
+      </c>
+      <c r="G23" s="1">
+        <v>83.1</v>
+      </c>
+      <c r="H23" s="1">
+        <v>1.66</v>
+      </c>
+      <c r="I23" s="2">
+        <f>E23/C$13</f>
+        <v>0.83098591549295775</v>
+      </c>
+      <c r="J23" s="2">
+        <f>F23/D$13</f>
+        <v>0.43693693693693691</v>
+      </c>
+      <c r="K23" s="2">
+        <f t="shared" si="4"/>
+        <v>0.39404897855602083</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>6</v>
+      </c>
+      <c r="B24" s="1">
+        <v>132</v>
+      </c>
+      <c r="C24" s="1">
+        <v>12</v>
+      </c>
+      <c r="D24" s="1">
+        <f t="shared" si="3"/>
+        <v>120</v>
+      </c>
+      <c r="E24" s="1">
+        <v>189</v>
+      </c>
+      <c r="F24" s="1">
+        <f t="shared" si="5"/>
+        <v>605</v>
+      </c>
+      <c r="G24" s="1">
+        <v>88.7</v>
+      </c>
+      <c r="H24" s="1">
+        <v>1.48</v>
+      </c>
+      <c r="I24" s="2">
+        <f>E24/C$13</f>
+        <v>0.88732394366197187</v>
+      </c>
+      <c r="J24" s="2">
+        <f>F24/D$13</f>
+        <v>0.54504504504504503</v>
+      </c>
+      <c r="K24" s="2">
+        <f t="shared" si="4"/>
+        <v>0.34227889861692684</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>7</v>
+      </c>
+      <c r="B25" s="1">
+        <v>133</v>
+      </c>
+      <c r="C25" s="1">
+        <v>5</v>
+      </c>
+      <c r="D25" s="1">
+        <f t="shared" si="3"/>
+        <v>128</v>
+      </c>
+      <c r="E25" s="1">
+        <v>194</v>
+      </c>
+      <c r="F25" s="1">
+        <f t="shared" si="5"/>
+        <v>733</v>
+      </c>
+      <c r="G25" s="1">
+        <v>91.1</v>
+      </c>
+      <c r="H25" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="I25" s="2">
+        <f>E25/C$13</f>
+        <v>0.91079812206572774</v>
+      </c>
+      <c r="J25" s="2">
+        <f>F25/D$13</f>
+        <v>0.66036036036036039</v>
+      </c>
+      <c r="K25" s="2">
+        <f t="shared" si="4"/>
+        <v>0.25043776170536736</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>8</v>
+      </c>
+      <c r="B26" s="1">
+        <v>132</v>
+      </c>
+      <c r="C26" s="1">
+        <v>10</v>
+      </c>
+      <c r="D26" s="1">
+        <f t="shared" si="3"/>
+        <v>122</v>
+      </c>
+      <c r="E26" s="1">
+        <v>204</v>
+      </c>
+      <c r="F26" s="1">
+        <f t="shared" si="5"/>
+        <v>855</v>
+      </c>
+      <c r="G26" s="1">
+        <v>95.8</v>
+      </c>
+      <c r="H26" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="I26" s="2">
+        <f>E26/C$13</f>
+        <v>0.95774647887323938</v>
+      </c>
+      <c r="J26" s="2">
+        <f>F26/D$13</f>
+        <v>0.77027027027027029</v>
+      </c>
+      <c r="K26" s="2">
+        <f t="shared" si="4"/>
+        <v>0.1874762086029691</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>9</v>
+      </c>
+      <c r="B27" s="1">
+        <v>132</v>
+      </c>
+      <c r="C27" s="1">
+        <v>3</v>
+      </c>
+      <c r="D27" s="1">
+        <f t="shared" si="3"/>
+        <v>129</v>
+      </c>
+      <c r="E27" s="1">
+        <v>207</v>
+      </c>
+      <c r="F27" s="1">
+        <f t="shared" si="5"/>
+        <v>984</v>
+      </c>
+      <c r="G27" s="1">
+        <v>97.2</v>
+      </c>
+      <c r="H27" s="1">
+        <v>1.08</v>
+      </c>
+      <c r="I27" s="2">
+        <f>E27/C$13</f>
+        <v>0.971830985915493</v>
+      </c>
+      <c r="J27" s="2">
+        <f>F27/D$13</f>
+        <v>0.88648648648648654</v>
+      </c>
+      <c r="K27" s="2">
+        <f t="shared" si="4"/>
+        <v>8.534449942900646E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>10</v>
+      </c>
+      <c r="B28" s="1">
+        <v>132</v>
+      </c>
+      <c r="C28" s="1">
+        <v>6</v>
+      </c>
+      <c r="D28" s="1">
+        <f t="shared" si="3"/>
+        <v>126</v>
+      </c>
+      <c r="E28" s="1">
         <v>213</v>
       </c>
+      <c r="F28" s="1">
+        <f t="shared" si="5"/>
+        <v>1110</v>
+      </c>
+      <c r="G28" s="1">
+        <v>100</v>
+      </c>
+      <c r="H28" s="1">
+        <v>1</v>
+      </c>
+      <c r="I28" s="2">
+        <f>E28/C$13</f>
+        <v>1</v>
+      </c>
+      <c r="J28" s="2">
+        <f>F28/D$13</f>
+        <v>1</v>
+      </c>
+      <c r="K28" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" s="1">
+        <f>SUM(B19:B28)</f>
+        <v>1323</v>
+      </c>
+      <c r="C29" s="16">
+        <f>SUM(C19:C28)</f>
+        <v>213</v>
+      </c>
+      <c r="D29" s="16">
+        <f>SUM(D19:D28)</f>
+        <v>1110</v>
+      </c>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A17:K17"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>